<commit_message>
🔧 Fix routes for front end display
</commit_message>
<xml_diff>
--- a/Project Plan 2025.xlsx
+++ b/Project Plan 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nrbes/Projects/ChatCommit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7A9304-5844-C244-B084-E41EA07A0B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6B7FA2-BEFA-294D-8A38-B7C18A3C7E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{50052AFE-25F9-724C-8834-CD92249D7E00}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>Component / Feature</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Commit bug fix (creation failure)</t>
-  </si>
-  <si>
-    <t>🐞 To Do</t>
   </si>
   <si>
     <t>Needs debugging + frontend feedback</t>
@@ -185,6 +182,27 @@
   </si>
   <si>
     <t>Post launch</t>
+  </si>
+  <si>
+    <t>To Do</t>
+  </si>
+  <si>
+    <t>Needs to be testted</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search by commit tags </t>
+  </si>
+  <si>
+    <t>User sign on? Or is that done through the settings in the extension?</t>
+  </si>
+  <si>
+    <t>Modify database to support accounts!</t>
+  </si>
+  <si>
+    <t>Working</t>
   </si>
 </sst>
 </file>
@@ -573,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19122A5-DE9C-FD49-8CE1-B9A309D9CF27}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,13 +662,13 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -661,7 +679,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -670,12 +688,12 @@
         <v>45749</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -687,194 +705,220 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>45751</v>
+      </c>
+      <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2">
-        <v>45751</v>
-      </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
-        <v>26</v>
+      <c r="E10" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C12">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2">
-        <v>45757</v>
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="C13">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2">
-        <v>45761</v>
+        <v>45757</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D14" s="2">
-        <v>45763</v>
+        <v>45761</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D15" s="2">
-        <v>45769</v>
+        <v>45763</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16" s="2">
-        <v>45771</v>
-      </c>
-      <c r="E16" t="s">
-        <v>39</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2">
+        <v>45769</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2">
+        <v>45771</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20" s="2">
+        <v>45773</v>
+      </c>
+      <c r="E20" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17" s="2">
-        <v>45773</v>
-      </c>
-      <c r="E17" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>